<commit_message>
TradingModel - 2021/11/15 watching updated
</commit_message>
<xml_diff>
--- a/TradingModel_OpenPositionWatching.xlsx
+++ b/TradingModel_OpenPositionWatching.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayWu\OneDrive - AAEON Technology\_OLD\Documents\Python\TradingModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaeon365-my.sharepoint.com/personal/raywu_aaeon_com_tw/Documents/_OLD/Documents/Python/TradingModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="14_{D8F70ED2-BD1C-4E29-871A-E650149FACE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6C1F1512-540D-450B-A778-467BFD0BD9B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{027A0A27-F260-4D45-95B2-C69F452D871A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14352" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15504" windowHeight="5868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,10 +427,16 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -472,28 +478,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1711</v>
+        <v>2436</v>
       </c>
       <c r="C2">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>27.15</v>
+        <v>204.8</v>
       </c>
       <c r="E2">
-        <v>5973</v>
+        <v>6020</v>
       </c>
       <c r="F2">
-        <v>27.3</v>
+        <v>88.9</v>
       </c>
       <c r="G2">
-        <v>24</v>
+        <v>66.8</v>
       </c>
       <c r="H2">
-        <v>29.35</v>
+        <v>88.9</v>
       </c>
       <c r="I2">
-        <v>27.5</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -501,28 +507,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2436</v>
+        <v>3035</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D3">
-        <v>99.3</v>
+        <v>185</v>
       </c>
       <c r="E3">
-        <v>4965</v>
+        <v>5920</v>
       </c>
       <c r="F3">
-        <v>88.9</v>
+        <v>121.5</v>
       </c>
       <c r="G3">
-        <v>66.8</v>
+        <v>86.7</v>
       </c>
       <c r="H3">
-        <v>88.9</v>
+        <v>176</v>
       </c>
       <c r="I3">
-        <v>66.8</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -530,28 +536,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3033</v>
+        <v>3122</v>
       </c>
       <c r="C4">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="D4">
-        <v>32.5</v>
+        <v>131</v>
       </c>
       <c r="E4">
-        <v>5850</v>
+        <v>5865</v>
       </c>
       <c r="F4">
-        <v>29.4</v>
+        <v>61.7</v>
       </c>
       <c r="G4">
-        <v>25.7</v>
+        <v>42.45</v>
       </c>
       <c r="H4">
-        <v>29.4</v>
+        <v>61.7</v>
       </c>
       <c r="I4">
-        <v>25.7</v>
+        <v>42.45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -559,28 +565,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3035</v>
+        <v>3141</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5">
+        <v>218.5</v>
+      </c>
+      <c r="E5">
+        <v>5899.5</v>
+      </c>
+      <c r="F5">
         <v>185</v>
       </c>
-      <c r="E5">
-        <v>5920</v>
-      </c>
-      <c r="F5">
-        <v>121.5</v>
-      </c>
       <c r="G5">
-        <v>86.7</v>
+        <v>127</v>
       </c>
       <c r="H5">
-        <v>176</v>
+        <v>237.5</v>
       </c>
       <c r="I5">
-        <v>163</v>
+        <v>213.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -588,28 +594,28 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3141</v>
+        <v>3588</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D6">
-        <v>218.5</v>
+        <v>155</v>
       </c>
       <c r="E6">
-        <v>5899.5</v>
+        <v>5425</v>
       </c>
       <c r="F6">
-        <v>185</v>
+        <v>142.5</v>
       </c>
       <c r="G6">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="H6">
-        <v>237.5</v>
+        <v>149</v>
       </c>
       <c r="I6">
-        <v>213.5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -617,28 +623,28 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3189</v>
+        <v>6104</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>235</v>
+        <v>170</v>
       </c>
       <c r="E7">
-        <v>6345</v>
+        <v>6120</v>
       </c>
       <c r="F7">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="G7">
-        <v>191</v>
+        <v>113.5</v>
       </c>
       <c r="H7">
-        <v>248</v>
+        <v>160</v>
       </c>
       <c r="I7">
-        <v>233</v>
+        <v>113.5</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -646,28 +652,28 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3588</v>
+        <v>6138</v>
       </c>
       <c r="C8">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8">
-        <v>155</v>
+        <v>203</v>
       </c>
       <c r="E8">
-        <v>5425</v>
+        <v>6090</v>
       </c>
       <c r="F8">
-        <v>142.5</v>
+        <v>193</v>
       </c>
       <c r="G8">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="H8">
-        <v>142.5</v>
+        <v>193</v>
       </c>
       <c r="I8">
-        <v>111</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -675,28 +681,28 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6104</v>
+        <v>6271</v>
       </c>
       <c r="C9">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>170</v>
+        <v>302.5</v>
       </c>
       <c r="E9">
-        <v>6120</v>
+        <v>6050</v>
       </c>
       <c r="F9">
-        <v>155</v>
+        <v>279.5</v>
       </c>
       <c r="G9">
-        <v>113.5</v>
+        <v>215.5</v>
       </c>
       <c r="H9">
-        <v>166.5</v>
+        <v>288</v>
       </c>
       <c r="I9">
-        <v>165.5</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -716,10 +722,10 @@
         <v>5980</v>
       </c>
       <c r="F10">
-        <v>227</v>
+        <v>222.5</v>
       </c>
       <c r="G10">
-        <v>190.5</v>
+        <v>180</v>
       </c>
       <c r="H10">
         <v>227</v>
@@ -736,21 +742,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068154D9CED6A274799344D73CDDB6092" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5a2665e4f307efafdee1c9405c7148c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0" xmlns:ns4="a05e4abd-8455-4909-9372-067b8b6e3dbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb69d6d218e7dc1efa9607e3a9562cb6" ns3:_="" ns4:_="">
     <xsd:import namespace="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
@@ -959,33 +950,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB6CFC54-CDBF-4A07-B3F2-16957552496F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{800E3977-04D6-441F-B515-43C1209344F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCB45FAA-C7B8-460C-8909-353D5DB6B841}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A2F3AF8-6081-4362-AA1B-DE7A6C9A8EAE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1001,4 +982,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0F19600-E6EB-4AE8-B4D4-57F1958D25E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D115C495-482F-4B78-A4FF-8E76798657E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>